<commit_message>
Plotted MI of toric code at different L with fixed p
</commit_message>
<xml_diff>
--- a/Toric_Code_MI.xlsx
+++ b/Toric_Code_MI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e00c848d2da39f20/Documents/3. Masters/Thesis/Code/MutualInfo/QEC_MI_MonteCarlo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="93" documentId="11_F25DC773A252ABDACC10485D899D72025ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A513F971-2DB5-4F0D-BA69-8A990208F2DB}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="13_ncr:1_{9A5585D8-8A4F-4623-B620-DF968991FFCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD5F672D-DF76-4A68-8A5C-560196B70D2B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -269,6 +269,975 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-AB86-42DF-BAAD-108D40A6F6E7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.02</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$10:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$10:$C$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0" formatCode="0.00E+00">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9469647069358002E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.8327729584790001E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.775648309713E-3</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00E+00">
+                  <c:v>5.4075658882470404E-4</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00E+00">
+                  <c:v>1.00915099402739E-4</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.00E+00">
+                  <c:v>1.7741470292799101E-5</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.00E+00">
+                  <c:v>5.1283983545504897E-6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-475D-4337-8AB0-630EEA324C6A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.03</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$18:$B$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$18:$C$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0" formatCode="0.00E+00">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.7054422594316003E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0907038408738001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.213663252473E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0128535592660001E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5118905946719999E-3</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.00E+00">
+                  <c:v>4.7784717083881298E-4</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.00E+00">
+                  <c:v>1.4228960712244301E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-828E-465F-984B-5C4A9FC2A090}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.04</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$26:$B$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$26:$C$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.7304518316994998E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.1110096248710003E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.9287786534580003E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.2722296810687E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.7738535953640002E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.2315702866390003E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5910-4685-B85A-7CB38B26E546}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.05</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$34:$B$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$34:$C$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.7250043807356006E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.8016611003536001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.11496090763049099</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.8193050369987004E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.8186202416707997E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BB46-4225-9E2A-C10237A3FBBF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$42</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.06</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$42:$B$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$42:$C$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.5387497229636006E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.5911977260143001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.21546985417654799</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.15426787600259101</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.10603706669995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E3F8-47E1-A435-3DDBF00940B3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$50</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.07</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$50:$B$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$50:$C$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.11101902811594599</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.6958719943003999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.34407189672881799</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.28473108708012701</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D08D-49A3-AFF3-9FA26224381C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$58</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.08</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$58:$B$65</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$58:$C$65</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.122309378847322</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0205007595013999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.487435982478575</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.44700534433073602</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4BD2-4308-86D9-489D9BEBD4AE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$66</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.09</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$66:$B$73</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$66:$C$73</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.130790334693972</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.5766467560434001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.63856778669556802</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.61809241705701801</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8666-4AEB-88BC-85F11D9FAF02}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$74</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$74:$B$81</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$74:$C$81</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.135175889057775</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-7.7339616387716997E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.75738215410623599</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8666-4AEB-88BC-85F11D9FAF02}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1161,16 +2130,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>22224</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>612399</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>69850</xdr:rowOff>
+      <xdr:rowOff>54907</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>457199</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>537881</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>134470</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1196,6 +2165,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1461,15 +2434,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AE14" sqref="AE14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1483,7 +2456,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0.01</v>
       </c>
@@ -1497,7 +2470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>0.01</v>
       </c>
@@ -1511,7 +2484,7 @@
         <v>1.0560102826176001E-6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>0.01</v>
       </c>
@@ -1525,7 +2498,7 @@
         <v>2.9557529979991501E-6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>0.01</v>
       </c>
@@ -1539,7 +2512,7 @@
         <v>5.76163987199594E-6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>0.01</v>
       </c>
@@ -1553,7 +2526,7 @@
         <v>1.0522043669013901E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>0.01</v>
       </c>
@@ -1567,7 +2540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>0.01</v>
       </c>
@@ -1581,7 +2554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>0.01</v>
       </c>
@@ -1595,67 +2568,905 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>0.02</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>0.02</v>
       </c>
       <c r="B11">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>1.9469647069358002E-2</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1.4276981602336E-6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>0.02</v>
       </c>
       <c r="B12">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>6.8327729584790001E-3</v>
+      </c>
+      <c r="D12" s="1">
+        <v>4.16459118692126E-6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>0.02</v>
       </c>
       <c r="B13">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>2.775648309713E-3</v>
+      </c>
+      <c r="D13" s="1">
+        <v>8.8201324026383393E-6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>0.02</v>
       </c>
       <c r="B14">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C14" s="1">
+        <v>5.4075658882470404E-4</v>
+      </c>
+      <c r="D14" s="1">
+        <v>6.1916436730808806E-5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>0.02</v>
       </c>
       <c r="B15">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15" s="1">
+        <v>1.00915099402739E-4</v>
+      </c>
+      <c r="D15" s="1">
+        <v>2.9833054885455E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>0.02</v>
       </c>
       <c r="B16">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" s="1">
+        <v>1.7741470292799101E-5</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1.1468660414117E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>0.02</v>
       </c>
       <c r="B17">
+        <v>15</v>
+      </c>
+      <c r="C17" s="1">
+        <v>5.1283983545504897E-6</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>0.03</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>0.03</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <v>3.7054422594316003E-2</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1.5860945126284601E-6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>0.03</v>
+      </c>
+      <c r="B20">
+        <v>5</v>
+      </c>
+      <c r="C20">
+        <v>2.0907038408738001E-2</v>
+      </c>
+      <c r="D20" s="1">
+        <v>4.7391900691068402E-6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>0.03</v>
+      </c>
+      <c r="B21">
+        <v>7</v>
+      </c>
+      <c r="C21">
+        <v>1.213663252473E-2</v>
+      </c>
+      <c r="D21" s="1">
+        <v>3.1431952782227902E-5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>0.03</v>
+      </c>
+      <c r="B22">
+        <v>9</v>
+      </c>
+      <c r="C22">
+        <v>5.0128535592660001E-3</v>
+      </c>
+      <c r="D22" s="1">
+        <v>3.3443434600204699E-5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>0.03</v>
+      </c>
+      <c r="B23">
+        <v>11</v>
+      </c>
+      <c r="C23">
+        <v>1.5118905946719999E-3</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1.0005706065740801E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>0.03</v>
+      </c>
+      <c r="B24">
+        <v>13</v>
+      </c>
+      <c r="C24" s="1">
+        <v>4.7784717083881298E-4</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>0.03</v>
+      </c>
+      <c r="B25">
+        <v>15</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1.4228960712244301E-4</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>0.04</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>0.04</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27">
+        <v>5.7304518316994998E-2</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1.6176099367402399E-6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>0.04</v>
+      </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="C28">
+        <v>4.1110096248710003E-2</v>
+      </c>
+      <c r="D28" s="1">
+        <v>5.1044900092238002E-6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>0.04</v>
+      </c>
+      <c r="B29">
+        <v>7</v>
+      </c>
+      <c r="C29">
+        <v>3.9287786534580003E-2</v>
+      </c>
+      <c r="D29" s="1">
+        <v>8.8326920819342997E-5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>0.04</v>
+      </c>
+      <c r="B30">
+        <v>9</v>
+      </c>
+      <c r="C30">
+        <v>2.2722296810687E-2</v>
+      </c>
+      <c r="D30" s="1">
+        <v>4.3810960777878198E-5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>0.04</v>
+      </c>
+      <c r="B31">
+        <v>11</v>
+      </c>
+      <c r="C31">
+        <v>9.7738535953640002E-3</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>0.04</v>
+      </c>
+      <c r="B32">
+        <v>13</v>
+      </c>
+      <c r="C32">
+        <v>4.2315702866390003E-3</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>0.04</v>
+      </c>
+      <c r="B33">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>0.05</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>0.05</v>
+      </c>
+      <c r="B35">
+        <v>3</v>
+      </c>
+      <c r="C35">
+        <v>7.7250043807356006E-2</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1.5657357238149901E-6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>0.05</v>
+      </c>
+      <c r="B36">
+        <v>5</v>
+      </c>
+      <c r="C36">
+        <v>5.8016611003536001E-2</v>
+      </c>
+      <c r="D36" s="1">
+        <v>5.3813938147043499E-6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>0.05</v>
+      </c>
+      <c r="B37">
+        <v>7</v>
+      </c>
+      <c r="C37">
+        <v>0.11496090763049099</v>
+      </c>
+      <c r="D37" s="1">
+        <v>1.9115885171345899E-5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>0.05</v>
+      </c>
+      <c r="B38">
+        <v>9</v>
+      </c>
+      <c r="C38">
+        <v>6.8193050369987004E-2</v>
+      </c>
+      <c r="D38" s="1">
+        <v>8.0503554303756295E-5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>0.05</v>
+      </c>
+      <c r="B39">
+        <v>11</v>
+      </c>
+      <c r="C39">
+        <v>3.8186202416707997E-2</v>
+      </c>
+      <c r="D39" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>0.05</v>
+      </c>
+      <c r="B40">
+        <v>13</v>
+      </c>
+      <c r="D40" s="1"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>0.05</v>
+      </c>
+      <c r="B41">
+        <v>15</v>
+      </c>
+      <c r="D41" s="1"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>0.06</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>0.06</v>
+      </c>
+      <c r="B43">
+        <v>3</v>
+      </c>
+      <c r="C43">
+        <v>9.5387497229636006E-2</v>
+      </c>
+      <c r="D43" s="1">
+        <v>1.45773727181605E-6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>0.06</v>
+      </c>
+      <c r="B44">
+        <v>5</v>
+      </c>
+      <c r="C44">
+        <v>6.5911977260143001E-2</v>
+      </c>
+      <c r="D44" s="1">
+        <v>5.50370927755115E-6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>0.06</v>
+      </c>
+      <c r="B45">
+        <v>7</v>
+      </c>
+      <c r="C45">
+        <v>0.21546985417654799</v>
+      </c>
+      <c r="D45" s="1">
+        <v>2.81636782010219E-5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>0.06</v>
+      </c>
+      <c r="B46">
+        <v>9</v>
+      </c>
+      <c r="C46">
+        <v>0.15426787600259101</v>
+      </c>
+      <c r="D46" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>0.06</v>
+      </c>
+      <c r="B47">
+        <v>11</v>
+      </c>
+      <c r="C47">
+        <v>0.10603706669995</v>
+      </c>
+      <c r="D47" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>0.06</v>
+      </c>
+      <c r="B48">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>0.06</v>
+      </c>
+      <c r="B49">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="B51">
+        <v>3</v>
+      </c>
+      <c r="C51">
+        <v>0.11101902811594599</v>
+      </c>
+      <c r="D51" s="1">
+        <v>1.3169325062390799E-6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="B52">
+        <v>5</v>
+      </c>
+      <c r="C52">
+        <v>5.6958719943003999E-2</v>
+      </c>
+      <c r="D52" s="1">
+        <v>5.5411319084789703E-6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="B53">
+        <v>7</v>
+      </c>
+      <c r="C53">
+        <v>0.34407189672881799</v>
+      </c>
+      <c r="D53" s="1">
+        <v>4.9750044368380101E-5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="B54">
+        <v>9</v>
+      </c>
+      <c r="C54">
+        <v>0.28473108708012701</v>
+      </c>
+      <c r="D54" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="B55">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="B56">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="B57">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <v>0.08</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>0.08</v>
+      </c>
+      <c r="B59">
+        <v>3</v>
+      </c>
+      <c r="C59">
+        <v>0.122309378847322</v>
+      </c>
+      <c r="D59" s="1">
+        <v>1.15940917182122E-6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>0.08</v>
+      </c>
+      <c r="B60">
+        <v>5</v>
+      </c>
+      <c r="C60">
+        <v>3.0205007595013999E-2</v>
+      </c>
+      <c r="D60" s="1">
+        <v>5.5564354891790197E-6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A61">
+        <v>0.08</v>
+      </c>
+      <c r="B61">
+        <v>7</v>
+      </c>
+      <c r="C61">
+        <v>0.487435982478575</v>
+      </c>
+      <c r="D61" s="1">
+        <v>1.2797068588997899E-4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A62">
+        <v>0.08</v>
+      </c>
+      <c r="B62">
+        <v>9</v>
+      </c>
+      <c r="C62">
+        <v>0.44700534433073602</v>
+      </c>
+      <c r="D62" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A63">
+        <v>0.08</v>
+      </c>
+      <c r="B63">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A64">
+        <v>0.08</v>
+      </c>
+      <c r="B64">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A65">
+        <v>0.08</v>
+      </c>
+      <c r="B65">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A66">
+        <v>0.09</v>
+      </c>
+      <c r="B66">
+        <v>1</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A67">
+        <v>0.09</v>
+      </c>
+      <c r="B67">
+        <v>3</v>
+      </c>
+      <c r="C67">
+        <v>0.130790334693972</v>
+      </c>
+      <c r="D67" s="1">
+        <v>9.9951422376969392E-7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A68">
+        <v>0.09</v>
+      </c>
+      <c r="B68">
+        <v>5</v>
+      </c>
+      <c r="C68">
+        <v>-1.5766467560434001E-2</v>
+      </c>
+      <c r="D68" s="1">
+        <v>5.5998122323610796E-6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A69">
+        <v>0.09</v>
+      </c>
+      <c r="B69">
+        <v>7</v>
+      </c>
+      <c r="C69">
+        <v>0.63856778669556802</v>
+      </c>
+      <c r="D69" s="1">
+        <v>7.9017578593570698E-5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A70">
+        <v>0.09</v>
+      </c>
+      <c r="B70">
+        <v>9</v>
+      </c>
+      <c r="C70">
+        <v>0.61809241705701801</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A71">
+        <v>0.09</v>
+      </c>
+      <c r="B71">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A72">
+        <v>0.09</v>
+      </c>
+      <c r="B72">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A73">
+        <v>0.09</v>
+      </c>
+      <c r="B73">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A74">
+        <v>0.1</v>
+      </c>
+      <c r="B74">
+        <v>1</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A75">
+        <v>0.1</v>
+      </c>
+      <c r="B75">
+        <v>3</v>
+      </c>
+      <c r="C75">
+        <v>0.135175889057775</v>
+      </c>
+      <c r="D75" s="1">
+        <v>8.4486346437766603E-7</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A76">
+        <v>0.1</v>
+      </c>
+      <c r="B76">
+        <v>5</v>
+      </c>
+      <c r="C76">
+        <v>-7.7339616387716997E-2</v>
+      </c>
+      <c r="D76" s="1">
+        <v>5.6512337494620401E-6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A77">
+        <v>0.1</v>
+      </c>
+      <c r="B77">
+        <v>7</v>
+      </c>
+      <c r="C77">
+        <v>0.75738215410623599</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A78">
+        <v>0.1</v>
+      </c>
+      <c r="B78">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A79">
+        <v>0.1</v>
+      </c>
+      <c r="B79">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A80">
+        <v>0.1</v>
+      </c>
+      <c r="B80">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A81">
+        <v>0.1</v>
+      </c>
+      <c r="B81">
         <v>15</v>
       </c>
     </row>

</xml_diff>